<commit_message>
Updated Aliases.xlsx, additional test report. Undone other changes to coincide with Thomas' requests.
</commit_message>
<xml_diff>
--- a/src/input_files/Aliases.xlsx
+++ b/src/input_files/Aliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mel91\Desktop\lew7\scheduler\src\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D235D1-18BB-4AC3-80BA-B13BB3C3F0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9B9C4F-BA68-491E-B081-ABE852C364AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18020" windowHeight="12220" xr2:uid="{58509038-36B9-C747-94F0-82C48A2EB557}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{58509038-36B9-C747-94F0-82C48A2EB557}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>CYBR 2160</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>CPSC 4115</t>
+  </si>
+  <si>
+    <t>CPSC 5115U</t>
   </si>
 </sst>
 </file>
@@ -411,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BD14FB-64A4-2C41-8B97-5CC7AF8EBE98}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -427,7 +430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -435,7 +438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -443,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -451,11 +454,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>